<commit_message>
Adding image documentsegmentation methods
</commit_message>
<xml_diff>
--- a/UnitTests/ComparingMethodsTest/TestFiles/Spreadsheet/excel_multi_no_break.xlsx
+++ b/UnitTests/ComparingMethodsTest/TestFiles/Spreadsheet/excel_multi_no_break.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaczm\Documents\bachelor\PROJECT\conv-file-quality-assurance\UnitTests\ComparingMethodsTest\TestFiles\Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFCB411-D6F4-49CF-8880-B9260C767D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB08FD1C-5345-420F-8ED3-319CE3BA0B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{35B7C187-9653-4A0C-BFB9-16F82C46E030}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId2"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="2">
   <si>
     <t>TEST</t>
   </si>
@@ -418,7 +418,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,26 +453,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F677FEC-6575-46E4-8040-29DEF121A3F3}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAEB3A0-838C-447F-A66A-93D3B7FC9DBC}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>